<commit_message>
Update ipa_map.py - interim
works for simple tests without role switchers and compound phones.
</commit_message>
<xml_diff>
--- a/src/ipa_features/IPA_Symbol_Table.xlsx
+++ b/src/ipa_features/IPA_Symbol_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcombiths/Documents/GitHub/ipa_features/src/ipa_features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B378D7-6154-FB45-AC7E-92B7AB7B2916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A84619-0436-1847-87C5-FCDFDBDAAC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="16480" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="1178">
   <si>
     <t>Description</t>
   </si>
@@ -3558,13 +3558,19 @@
     <t>0x2205</t>
   </si>
   <si>
-    <t>suprasegmental</t>
-  </si>
-  <si>
     <t>diacritic_role-switcher</t>
   </si>
   <si>
     <t>Role</t>
+  </si>
+  <si>
+    <t>compound_right</t>
+  </si>
+  <si>
+    <t>stress</t>
+  </si>
+  <si>
+    <t>boundary</t>
   </si>
 </sst>
 </file>
@@ -4165,7 +4171,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4176,6 +4182,7 @@
     <col min="4" max="4" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="13" width="12.33203125" customWidth="1"/>
@@ -4203,7 +4210,7 @@
         <v>1021</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1022</v>
@@ -10413,7 +10420,7 @@
         <v>1014</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="H122" t="str">
         <f t="shared" si="26"/>
@@ -10440,7 +10447,7 @@
         <v>1014</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>1173</v>
+        <v>1176</v>
       </c>
       <c r="H123" t="str">
         <f t="shared" si="26"/>
@@ -10494,7 +10501,7 @@
         <v>1014</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>1074</v>
+        <v>1175</v>
       </c>
       <c r="H125" t="str">
         <f t="shared" si="26"/>
@@ -10521,7 +10528,7 @@
         <v>1014</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>1074</v>
+        <v>1175</v>
       </c>
       <c r="H126" t="str">
         <f t="shared" si="26"/>
@@ -10548,7 +10555,7 @@
         <v>1014</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>1173</v>
+        <v>1177</v>
       </c>
       <c r="H127" t="str">
         <f t="shared" si="26"/>
@@ -10575,7 +10582,7 @@
         <v>1014</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>1173</v>
+        <v>1177</v>
       </c>
       <c r="H128" t="str">
         <f t="shared" si="26"/>
@@ -10629,7 +10636,7 @@
         <v>1014</v>
       </c>
       <c r="G130" s="1" t="s">
-        <v>1173</v>
+        <v>1177</v>
       </c>
       <c r="H130" t="str">
         <f t="shared" si="26"/>
@@ -11329,7 +11336,7 @@
         <v>1017</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="H156" t="str">
         <f t="shared" si="27"/>

</xml_diff>

<commit_message>
added two last rows to IPA_Symbol_Table manually
</commit_message>
<xml_diff>
--- a/src/ipa_features/IPA_Symbol_Table.xlsx
+++ b/src/ipa_features/IPA_Symbol_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcombiths/Documents/GitHub/ipa_features/src/ipa_features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A84619-0436-1847-87C5-FCDFDBDAAC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6DEBC-0F43-B747-AB3C-76220CF6E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="16480" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="16380" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
   </bookViews>
   <sheets>
     <sheet name="IPA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="1178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="1186">
   <si>
     <t>Description</t>
   </si>
@@ -3571,6 +3571,30 @@
   </si>
   <si>
     <t>boundary</t>
+  </si>
+  <si>
+    <t>̴</t>
+  </si>
+  <si>
+    <t>0x334</t>
+  </si>
+  <si>
+    <t>COMBINING TILDE OVERLAY</t>
+  </si>
+  <si>
+    <t>0x03A</t>
+  </si>
+  <si>
+    <t>NON-SPACING RING ABOVE</t>
+  </si>
+  <si>
+    <t>̊</t>
+  </si>
+  <si>
+    <t>̴̴</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
   </si>
 </sst>
 </file>
@@ -3805,8 +3829,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X260" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:X260" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X262" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:X262" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{634E2ACC-F650-4879-A647-12FAF9317E57}" name="Description" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{BAEC8A6F-34A0-4732-BD0F-2F751D247EC8}" name="Name" dataDxfId="5"/>
@@ -4167,11 +4191,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E616C57-35B6-46C5-A285-FD5E9EF1060B}">
-  <dimension ref="A1:X260"/>
+  <dimension ref="A1:X262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D262" sqref="D262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14136,6 +14160,60 @@
       </c>
       <c r="H260" t="str">
         <f>IF(ISNUMBER(SEARCH("Voiceless",A260)),0, IF(ISNUMBER(SEARCH("Voiced",A260)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F261" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G261" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H261" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A261)),0, IF(ISNUMBER(SEARCH("Voiced",A261)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>1183</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F262" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G262" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H262" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A262)),0, IF(ISNUMBER(SEARCH("Voiced",A262)),1,""))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
manual add to IPA_Symbol_Table
</commit_message>
<xml_diff>
--- a/src/ipa_features/IPA_Symbol_Table.xlsx
+++ b/src/ipa_features/IPA_Symbol_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pcombiths/Documents/GitHub/ipa_features/src/ipa_features/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6DEBC-0F43-B747-AB3C-76220CF6E0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18141DB5-71D3-B448-B289-C2BA8BB33166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="29400" windowHeight="16380" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="IPA" sheetId="1" r:id="rId1"/>
     <sheet name="features_ref" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3826" uniqueCount="1186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3844" uniqueCount="1195">
   <si>
     <t>Description</t>
   </si>
@@ -3595,13 +3595,40 @@
   </si>
   <si>
     <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>ᵈ</t>
+  </si>
+  <si>
+    <t>superscript D</t>
+  </si>
+  <si>
+    <t>Modifier letter small D</t>
+  </si>
+  <si>
+    <t>0x0064</t>
+  </si>
+  <si>
+    <t>ᵗ</t>
+  </si>
+  <si>
+    <t>Modifier letter small T</t>
+  </si>
+  <si>
+    <t>superscript T</t>
+  </si>
+  <si>
+    <t>0x0074</t>
+  </si>
+  <si>
+    <t>ᶷ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3626,6 +3653,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3648,7 +3681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3657,6 +3690,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3829,8 +3863,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X262" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:X262" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X265" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:X265" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{634E2ACC-F650-4879-A647-12FAF9317E57}" name="Description" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{BAEC8A6F-34A0-4732-BD0F-2F751D247EC8}" name="Name" dataDxfId="5"/>
@@ -4191,11 +4225,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E616C57-35B6-46C5-A285-FD5E9EF1060B}">
-  <dimension ref="A1:X262"/>
+  <dimension ref="A1:X265"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D262" sqref="D262"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B264" sqref="B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14214,6 +14248,81 @@
       </c>
       <c r="H262" t="str">
         <f>IF(ISNUMBER(SEARCH("Voiceless",A262)),0, IF(ISNUMBER(SEARCH("Voiced",A262)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="F263" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G263" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H263" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A263)),0, IF(ISNUMBER(SEARCH("Voiced",A263)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="264" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D264" s="4" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F264" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G264" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H264" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A264)),0, IF(ISNUMBER(SEARCH("Voiced",A264)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265" s="1"/>
+      <c r="B265" s="1"/>
+      <c r="C265" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E265" s="1"/>
+      <c r="F265" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="G265" s="1" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H265" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A265)),0, IF(ISNUMBER(SEARCH("Voiced",A265)),1,""))</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Added cover symbol *
</commit_message>
<xml_diff>
--- a/src/ipa_features/IPA_Symbol_Table.xlsx
+++ b/src/ipa_features/IPA_Symbol_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pcombiths\Documents\github\ipa_features\src\ipa_features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C5BF51-E14A-4AC2-919A-FB40EECD4310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA680E07-42C4-455B-A489-FCC2DB711B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1395" windowWidth="29010" windowHeight="15345" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
+    <workbookView xWindow="76680" yWindow="-3255" windowWidth="29040" windowHeight="15720" xr2:uid="{6C036820-CBD9-4851-A4E3-4573182BB3A6}"/>
   </bookViews>
   <sheets>
     <sheet name="IPA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3904" uniqueCount="1242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3910" uniqueCount="1245">
   <si>
     <t>Description</t>
   </si>
@@ -3763,6 +3763,15 @@
   </si>
   <si>
     <t>˃</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Unintelligible cover symbol</t>
+  </si>
+  <si>
+    <t>unintelligible cover symbol</t>
   </si>
 </sst>
 </file>
@@ -3997,8 +4006,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X273" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:X273" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D043D4FE-F354-4BBC-9B2E-170C38C7EE75}" name="Table1" displayName="Table1" ref="A1:X274" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:X274" xr:uid="{0D396139-44B1-4D2F-ADA9-6F97CAD5E738}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{634E2ACC-F650-4879-A647-12FAF9317E57}" name="Description" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{BAEC8A6F-34A0-4732-BD0F-2F751D247EC8}" name="Name" dataDxfId="5"/>
@@ -4359,11 +4368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E616C57-35B6-46C5-A285-FD5E9EF1060B}">
-  <dimension ref="A1:X273"/>
+  <dimension ref="A1:X274"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E222" sqref="E222"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D271" sqref="D271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14681,6 +14690,31 @@
       </c>
       <c r="H273" t="str">
         <f>IF(ISNUMBER(SEARCH("Voiceless",A273)),0, IF(ISNUMBER(SEARCH("Voiced",A273)),1,""))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E274" s="1"/>
+      <c r="F274" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G274" s="1" t="s">
+        <v>1073</v>
+      </c>
+      <c r="H274" t="str">
+        <f>IF(ISNUMBER(SEARCH("Voiceless",A274)),0, IF(ISNUMBER(SEARCH("Voiced",A274)),1,""))</f>
         <v/>
       </c>
     </row>

</xml_diff>